<commit_message>
crear la funcion de agregar tarea
</commit_message>
<xml_diff>
--- a/hojaDatos.xlsx
+++ b/hojaDatos.xlsx
@@ -1,76 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mi unidad\Sena\Danilo\git-flow en grupo\git-flow\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE23207-AEC7-4C53-8771-9DD43F164998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="tareas" sheetId="1" r:id="rId1"/>
-    <sheet name="productos" sheetId="2" r:id="rId2"/>
+    <sheet name="tareas" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="productos" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>descripcion</t>
-  </si>
-  <si>
-    <t>estado</t>
-  </si>
-  <si>
-    <t>fecha_inicio</t>
-  </si>
-  <si>
-    <t>fecha_fin</t>
-  </si>
-  <si>
-    <t>categoria</t>
-  </si>
-  <si>
-    <t>precio</t>
-  </si>
-  <si>
-    <t>cantidad</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -89,24 +47,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -372,41 +389,147 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col width="4.85546875" customWidth="1" min="1" max="1"/>
+    <col width="9.140625" customWidth="1" min="2" max="2"/>
+    <col width="13.42578125" customWidth="1" min="3" max="3"/>
+    <col width="7.140625" customWidth="1" min="4" max="4"/>
+    <col width="12.5703125" customWidth="1" min="5" max="5"/>
+    <col width="11.5703125" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>nombre</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>descripcion</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>estado</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>fecha_inicio</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>fecha_fin</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>lili</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>sdadsadas</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>pendiente</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>12/02/2023</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>13/02/2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>lili</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>sdadsadas</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>pendiente</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>12/02/2023</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>13/02/2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>lili</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>sdadsadas</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>pendiente</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>12/02/2023</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>13/02/2023</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -415,30 +538,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD5B45E-78E9-4423-BB0B-E4216DECBA66}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="A1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>nombre</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>categoria</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>precio</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>cantidad</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
creacion de la funcion actualizar tarea
</commit_message>
<xml_diff>
--- a/hojaDatos.xlsx
+++ b/hojaDatos.xlsx
@@ -1,76 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mi unidad\Sena\Danilo\git-flow en grupo\git-flow\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE23207-AEC7-4C53-8771-9DD43F164998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3036" yWindow="2820" windowWidth="17280" windowHeight="9420" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="tareas" sheetId="1" r:id="rId1"/>
-    <sheet name="productos" sheetId="2" r:id="rId2"/>
+    <sheet name="tareas" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="productos" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>descripcion</t>
-  </si>
-  <si>
-    <t>estado</t>
-  </si>
-  <si>
-    <t>fecha_inicio</t>
-  </si>
-  <si>
-    <t>fecha_fin</t>
-  </si>
-  <si>
-    <t>categoria</t>
-  </si>
-  <si>
-    <t>precio</t>
-  </si>
-  <si>
-    <t>cantidad</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -89,24 +47,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -372,41 +389,87 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col width="4.88671875" customWidth="1" min="1" max="1"/>
+    <col width="9.109375" customWidth="1" min="2" max="2"/>
+    <col width="13.44140625" customWidth="1" min="3" max="3"/>
+    <col width="7.109375" customWidth="1" min="4" max="4"/>
+    <col width="12.5546875" customWidth="1" min="5" max="5"/>
+    <col width="11.5546875" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>nombre</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>descripcion</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>estado</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>fecha_inicio</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>fecha_fin</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>yoiner</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>sdasdsadas</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>pendiente</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>12/2/2023</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>12/2/2023</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -415,30 +478,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD5B45E-78E9-4423-BB0B-E4216DECBA66}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="A1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>nombre</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>categoria</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>precio</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>cantidad</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
crear archivo crud de los productos
</commit_message>
<xml_diff>
--- a/hojaDatos.xlsx
+++ b/hojaDatos.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mi unidad\Sena\Danilo\git-flow en grupo\git-flow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sakur\OneDrive\Escritorio\gitflow\git-flow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE23207-AEC7-4C53-8771-9DD43F164998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tareas" sheetId="1" r:id="rId1"/>
     <sheet name="productos" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>id</t>
   </si>
@@ -53,12 +52,18 @@
   </si>
   <si>
     <t>cantidad</t>
+  </si>
+  <si>
+    <t>roa</t>
+  </si>
+  <si>
+    <t>cereal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -372,10 +377,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -415,11 +420,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD5B45E-78E9-4423-BB0B-E4216DECBA66}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,6 +446,23 @@
         <v>8</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>2500</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
creacion de la funcion de agregar productos
</commit_message>
<xml_diff>
--- a/hojaDatos.xlsx
+++ b/hojaDatos.xlsx
@@ -1,81 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sakur\OneDrive\Escritorio\gitflow\git-flow\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="tareas" sheetId="1" r:id="rId1"/>
-    <sheet name="productos" sheetId="2" r:id="rId2"/>
+    <sheet name="tareas" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="productos" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="152511" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>descripcion</t>
-  </si>
-  <si>
-    <t>estado</t>
-  </si>
-  <si>
-    <t>fecha_inicio</t>
-  </si>
-  <si>
-    <t>fecha_fin</t>
-  </si>
-  <si>
-    <t>categoria</t>
-  </si>
-  <si>
-    <t>precio</t>
-  </si>
-  <si>
-    <t>cantidad</t>
-  </si>
-  <si>
-    <t>roa</t>
-  </si>
-  <si>
-    <t>cereal</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -94,24 +47,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -377,41 +389,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col width="4.85546875" customWidth="1" min="1" max="1"/>
+    <col width="9.140625" customWidth="1" min="2" max="2"/>
+    <col width="13.42578125" customWidth="1" min="3" max="3"/>
+    <col width="7.140625" customWidth="1" min="4" max="4"/>
+    <col width="12.5703125" customWidth="1" min="5" max="5"/>
+    <col width="11.5703125" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>nombre</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>descripcion</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>estado</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>fecha_inicio</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>fecha_fin</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -420,47 +448,86 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>nombre</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>categoria</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>precio</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>cantidad</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>roa</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>cereal</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>2500</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>2500</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>cafe</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>grano</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
creacion de la funcion de actualizar productos
</commit_message>
<xml_diff>
--- a/hojaDatos.xlsx
+++ b/hojaDatos.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mi unidad\Sena\Danilo\git-flow en grupo\git-flow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE23207-AEC7-4C53-8771-9DD43F164998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61D3ADC-4EC2-4AB3-8753-A22F4ACCDA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tareas" sheetId="1" r:id="rId1"/>
     <sheet name="productos" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -375,7 +370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -415,11 +410,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD5B45E-78E9-4423-BB0B-E4216DECBA66}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>